<commit_message>
Add styling support for strong tags in Excel export
</commit_message>
<xml_diff>
--- a/Output Test.xlsx
+++ b/Output Test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_9A3D87D842DA09F27A57B5BF012BA6C47D31C154" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A63B6393-D148-4148-9E52-983887188A90}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_9A3D87D842DA09F27A57B5BF012BA6C47D31C154" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CD46496-2C0A-419D-9979-B72BD50D7CBF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1455,6 +1455,38 @@
     <t>Idol Dream</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Invoke: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Restore </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> health to your hero.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Overhealed</t>
+    </r>
+  </si>
+  <si>
     <t>Slice of Heaven</t>
   </si>
   <si>
@@ -4606,31 +4638,6 @@
   </si>
   <si>
     <t>X01</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">Invoke: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Restore  health to your hero.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Overhealed</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -21680,7 +21687,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -22581,8 +22588,8 @@
       <c r="F21" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="110" t="s">
-        <v>520</v>
+      <c r="G21" s="28" t="s">
+        <v>242</v>
       </c>
       <c r="H21" s="31" t="s">
         <v>15</v>
@@ -22611,10 +22618,10 @@
         <v>35</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D22" s="28" t="s">
         <v>15</v>
@@ -22626,7 +22633,7 @@
         <v>15</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="H22" s="31" t="s">
         <v>15</v>
@@ -22652,7 +22659,7 @@
     </row>
     <row r="23" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B23" s="26" t="s">
         <v>15</v>
@@ -22735,7 +22742,7 @@
         <v>39</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C25" s="27" t="s">
         <v>186</v>
@@ -22747,10 +22754,10 @@
         <v>1</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>247</v>
-      </c>
-      <c r="G25" s="28" t="s">
         <v>248</v>
+      </c>
+      <c r="G25" s="110" t="s">
+        <v>249</v>
       </c>
       <c r="H25" s="31" t="s">
         <v>15</v>
@@ -22779,7 +22786,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C26" s="27" t="s">
         <v>186</v>
@@ -22791,13 +22798,13 @@
         <v>1</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G26" s="28" t="s">
         <v>16</v>
       </c>
       <c r="H26" s="31" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="I26" s="28"/>
       <c r="J26" s="27"/>
@@ -22823,7 +22830,7 @@
         <v>41</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C27" s="27" t="s">
         <v>186</v>
@@ -22835,10 +22842,10 @@
         <v>1</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G27" s="28" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H27" s="31" t="s">
         <v>15</v>
@@ -22867,13 +22874,13 @@
         <v>42</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C28" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E28" s="29">
         <v>2</v>
@@ -22882,10 +22889,10 @@
         <v>188</v>
       </c>
       <c r="G28" s="28" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H28" s="31" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="I28" s="28"/>
       <c r="J28" s="27"/>
@@ -22911,7 +22918,7 @@
         <v>43</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C29" s="27" t="s">
         <v>186</v>
@@ -22923,10 +22930,10 @@
         <v>2</v>
       </c>
       <c r="F29" s="30" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G29" s="28" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H29" s="31" t="s">
         <v>15</v>
@@ -22955,22 +22962,22 @@
         <v>44</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C30" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D30" s="28" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E30" s="29">
         <v>3</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G30" s="28" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H30" s="31" t="s">
         <v>15</v>
@@ -22999,7 +23006,7 @@
         <v>45</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C31" s="27" t="s">
         <v>186</v>
@@ -23011,10 +23018,10 @@
         <v>3</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G31" s="28" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H31" s="31" t="s">
         <v>15</v>
@@ -23043,7 +23050,7 @@
         <v>46</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>186</v>
@@ -23058,7 +23065,7 @@
         <v>200</v>
       </c>
       <c r="G32" s="28" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="H32" s="31" t="s">
         <v>15</v>
@@ -23087,7 +23094,7 @@
         <v>47</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C33" s="27" t="s">
         <v>186</v>
@@ -23099,10 +23106,10 @@
         <v>4</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G33" s="28" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H33" s="31" t="s">
         <v>15</v>
@@ -23131,7 +23138,7 @@
         <v>48</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>186</v>
@@ -23143,10 +23150,10 @@
         <v>4</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G34" s="28" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H34" s="31" t="s">
         <v>202</v>
@@ -23175,7 +23182,7 @@
         <v>49</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C35" s="27" t="s">
         <v>186</v>
@@ -23190,7 +23197,7 @@
         <v>218</v>
       </c>
       <c r="G35" s="28" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="H35" s="31" t="s">
         <v>15</v>
@@ -23219,22 +23226,22 @@
         <v>50</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C36" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D36" s="28" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E36" s="29">
         <v>5</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G36" s="28" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H36" s="31" t="s">
         <v>15</v>
@@ -23263,7 +23270,7 @@
         <v>51</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C37" s="27" t="s">
         <v>186</v>
@@ -23275,10 +23282,10 @@
         <v>6</v>
       </c>
       <c r="F37" s="30" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="G37" s="28" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H37" s="31" t="s">
         <v>202</v>
@@ -23307,7 +23314,7 @@
         <v>52</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>186</v>
@@ -23319,10 +23326,10 @@
         <v>7</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G38" s="28" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H38" s="31" t="s">
         <v>15</v>
@@ -23351,7 +23358,7 @@
         <v>53</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C39" s="27" t="s">
         <v>225</v>
@@ -23366,7 +23373,7 @@
         <v>15</v>
       </c>
       <c r="G39" s="28" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H39" s="31" t="s">
         <v>15</v>
@@ -23395,7 +23402,7 @@
         <v>54</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C40" s="27" t="s">
         <v>225</v>
@@ -23410,7 +23417,7 @@
         <v>15</v>
       </c>
       <c r="G40" s="28" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="H40" s="31" t="s">
         <v>15</v>
@@ -23439,7 +23446,7 @@
         <v>55</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C41" s="27" t="s">
         <v>225</v>
@@ -23454,7 +23461,7 @@
         <v>15</v>
       </c>
       <c r="G41" s="28" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="H41" s="31" t="s">
         <v>15</v>
@@ -23483,7 +23490,7 @@
         <v>56</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C42" s="27" t="s">
         <v>173</v>
@@ -23498,7 +23505,7 @@
         <v>15</v>
       </c>
       <c r="G42" s="28" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="H42" s="31" t="s">
         <v>15</v>
@@ -23527,25 +23534,25 @@
         <v>57</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D43" s="28" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E43" s="29">
         <v>2</v>
       </c>
       <c r="F43" s="30" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G43" s="28" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H43" s="31" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="I43" s="28"/>
       <c r="J43" s="27"/>
@@ -23571,10 +23578,10 @@
         <v>58</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D44" s="28" t="s">
         <v>15</v>
@@ -23586,7 +23593,7 @@
         <v>192</v>
       </c>
       <c r="G44" s="28" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H44" s="31" t="s">
         <v>15</v>
@@ -23612,7 +23619,7 @@
     </row>
     <row r="45" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B45" s="26" t="s">
         <v>15</v>
@@ -23695,22 +23702,22 @@
         <v>62</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C47" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D47" s="28" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E47" s="29">
         <v>1</v>
       </c>
       <c r="F47" s="30" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G47" s="28" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="H47" s="31" t="s">
         <v>15</v>
@@ -23739,7 +23746,7 @@
         <v>63</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C48" s="27" t="s">
         <v>186</v>
@@ -23751,10 +23758,10 @@
         <v>1</v>
       </c>
       <c r="F48" s="30" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G48" s="28" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="H48" s="31" t="s">
         <v>15</v>
@@ -23783,13 +23790,13 @@
         <v>64</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C49" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E49" s="29">
         <v>1</v>
@@ -23798,10 +23805,10 @@
         <v>188</v>
       </c>
       <c r="G49" s="28" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H49" s="31" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="I49" s="28"/>
       <c r="J49" s="27"/>
@@ -23827,7 +23834,7 @@
         <v>65</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C50" s="27" t="s">
         <v>186</v>
@@ -23839,10 +23846,10 @@
         <v>2</v>
       </c>
       <c r="F50" s="30" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G50" s="28" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="H50" s="31" t="s">
         <v>15</v>
@@ -23871,7 +23878,7 @@
         <v>66</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C51" s="27" t="s">
         <v>186</v>
@@ -23886,7 +23893,7 @@
         <v>192</v>
       </c>
       <c r="G51" s="28" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H51" s="31" t="s">
         <v>15</v>
@@ -23915,22 +23922,22 @@
         <v>67</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C52" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E52" s="29">
         <v>3</v>
       </c>
       <c r="F52" s="30" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G52" s="28" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="H52" s="31" t="s">
         <v>15</v>
@@ -23959,22 +23966,22 @@
         <v>68</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C53" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E53" s="29">
         <v>4</v>
       </c>
       <c r="F53" s="30" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="G53" s="28" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="H53" s="31" t="s">
         <v>15</v>
@@ -24003,7 +24010,7 @@
         <v>69</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C54" s="27" t="s">
         <v>186</v>
@@ -24015,10 +24022,10 @@
         <v>5</v>
       </c>
       <c r="F54" s="30" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="G54" s="28" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="H54" s="31" t="s">
         <v>15</v>
@@ -24047,22 +24054,22 @@
         <v>70</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C55" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D55" s="28" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="E55" s="29">
         <v>15</v>
       </c>
       <c r="F55" s="30" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G55" s="28" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="H55" s="31" t="s">
         <v>15</v>
@@ -24091,13 +24098,13 @@
         <v>71</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C56" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D56" s="28" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E56" s="29">
         <v>1</v>
@@ -24106,7 +24113,7 @@
         <v>15</v>
       </c>
       <c r="G56" s="28" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="H56" s="31" t="s">
         <v>15</v>
@@ -24135,13 +24142,13 @@
         <v>72</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C57" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D57" s="28" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E57" s="29">
         <v>1</v>
@@ -24150,7 +24157,7 @@
         <v>15</v>
       </c>
       <c r="G57" s="28" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="H57" s="31" t="s">
         <v>15</v>
@@ -24179,13 +24186,13 @@
         <v>73</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C58" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E58" s="29">
         <v>1</v>
@@ -24194,7 +24201,7 @@
         <v>15</v>
       </c>
       <c r="G58" s="28" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="H58" s="31" t="s">
         <v>15</v>
@@ -24223,13 +24230,13 @@
         <v>74</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C59" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D59" s="28" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E59" s="29">
         <v>2</v>
@@ -24238,7 +24245,7 @@
         <v>15</v>
       </c>
       <c r="G59" s="28" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="H59" s="31" t="s">
         <v>15</v>
@@ -24267,13 +24274,13 @@
         <v>75</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C60" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D60" s="28" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E60" s="29">
         <v>2</v>
@@ -24282,7 +24289,7 @@
         <v>15</v>
       </c>
       <c r="G60" s="28" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="H60" s="31" t="s">
         <v>15</v>
@@ -24311,13 +24318,13 @@
         <v>76</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C61" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D61" s="28" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E61" s="29">
         <v>3</v>
@@ -24326,7 +24333,7 @@
         <v>15</v>
       </c>
       <c r="G61" s="28" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="H61" s="31" t="s">
         <v>15</v>
@@ -24355,7 +24362,7 @@
         <v>77</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C62" s="27" t="s">
         <v>225</v>
@@ -24370,7 +24377,7 @@
         <v>15</v>
       </c>
       <c r="G62" s="28" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="H62" s="31" t="s">
         <v>15</v>
@@ -24399,7 +24406,7 @@
         <v>78</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C63" s="27" t="s">
         <v>173</v>
@@ -24414,7 +24421,7 @@
         <v>15</v>
       </c>
       <c r="G63" s="28" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="H63" s="31" t="s">
         <v>15</v>
@@ -24443,13 +24450,13 @@
         <v>79</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C64" s="27" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D64" s="28" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E64" s="29">
         <v>2</v>
@@ -24487,22 +24494,22 @@
         <v>80</v>
       </c>
       <c r="B65" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="C65" s="27" t="s">
+        <v>296</v>
+      </c>
+      <c r="D65" s="28" t="s">
         <v>349</v>
-      </c>
-      <c r="C65" s="27" t="s">
-        <v>295</v>
-      </c>
-      <c r="D65" s="28" t="s">
-        <v>348</v>
       </c>
       <c r="E65" s="29">
         <v>2</v>
       </c>
       <c r="F65" s="30" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G65" s="28" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="H65" s="31" t="s">
         <v>15</v>
@@ -24531,10 +24538,10 @@
         <v>81</v>
       </c>
       <c r="B66" s="26" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C66" s="27" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D66" s="28" t="s">
         <v>15</v>
@@ -24546,7 +24553,7 @@
         <v>15</v>
       </c>
       <c r="G66" s="28" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="H66" s="31" t="s">
         <v>15</v>
@@ -24572,7 +24579,7 @@
     </row>
     <row r="67" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="97" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B67" s="26" t="s">
         <v>15</v>
@@ -24655,7 +24662,7 @@
         <v>85</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C69" s="27" t="s">
         <v>186</v>
@@ -24670,7 +24677,7 @@
         <v>188</v>
       </c>
       <c r="G69" s="28" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="H69" s="31" t="s">
         <v>15</v>
@@ -24699,7 +24706,7 @@
         <v>86</v>
       </c>
       <c r="B70" s="26" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C70" s="27" t="s">
         <v>186</v>
@@ -24714,10 +24721,10 @@
         <v>188</v>
       </c>
       <c r="G70" s="28" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="H70" s="31" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="I70" s="28"/>
       <c r="J70" s="27"/>
@@ -24743,7 +24750,7 @@
         <v>87</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C71" s="27" t="s">
         <v>186</v>
@@ -24755,13 +24762,13 @@
         <v>2</v>
       </c>
       <c r="F71" s="30" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G71" s="28" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="H71" s="31" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="I71" s="28"/>
       <c r="J71" s="27"/>
@@ -24787,7 +24794,7 @@
         <v>88</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C72" s="27" t="s">
         <v>186</v>
@@ -24802,7 +24809,7 @@
         <v>196</v>
       </c>
       <c r="G72" s="28" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="H72" s="31" t="s">
         <v>15</v>
@@ -24831,7 +24838,7 @@
         <v>89</v>
       </c>
       <c r="B73" s="26" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C73" s="27" t="s">
         <v>186</v>
@@ -24843,10 +24850,10 @@
         <v>2</v>
       </c>
       <c r="F73" s="30" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="G73" s="28" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="H73" s="31" t="s">
         <v>202</v>
@@ -24875,13 +24882,13 @@
         <v>90</v>
       </c>
       <c r="B74" s="26" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C74" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D74" s="28" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E74" s="29">
         <v>2</v>
@@ -24890,7 +24897,7 @@
         <v>196</v>
       </c>
       <c r="G74" s="28" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="H74" s="31" t="s">
         <v>15</v>
@@ -24919,13 +24926,13 @@
         <v>91</v>
       </c>
       <c r="B75" s="26" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C75" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D75" s="28" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E75" s="29">
         <v>3</v>
@@ -24934,7 +24941,7 @@
         <v>192</v>
       </c>
       <c r="G75" s="28" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="H75" s="31" t="s">
         <v>15</v>
@@ -24963,7 +24970,7 @@
         <v>92</v>
       </c>
       <c r="B76" s="26" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C76" s="27" t="s">
         <v>186</v>
@@ -24978,7 +24985,7 @@
         <v>200</v>
       </c>
       <c r="G76" s="28" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="H76" s="31" t="s">
         <v>202</v>
@@ -25007,22 +25014,22 @@
         <v>93</v>
       </c>
       <c r="B77" s="26" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C77" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D77" s="28" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E77" s="29">
         <v>5</v>
       </c>
       <c r="F77" s="30" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="G77" s="28" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="H77" s="31" t="s">
         <v>15</v>
@@ -25051,7 +25058,7 @@
         <v>94</v>
       </c>
       <c r="B78" s="26" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C78" s="27" t="s">
         <v>186</v>
@@ -25063,10 +25070,10 @@
         <v>5</v>
       </c>
       <c r="F78" s="30" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="G78" s="28" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H78" s="31" t="s">
         <v>15</v>
@@ -25095,13 +25102,13 @@
         <v>95</v>
       </c>
       <c r="B79" s="26" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C79" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D79" s="28" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E79" s="29">
         <v>1</v>
@@ -25110,7 +25117,7 @@
         <v>15</v>
       </c>
       <c r="G79" s="28" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="H79" s="31" t="s">
         <v>15</v>
@@ -25139,13 +25146,13 @@
         <v>96</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C80" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E80" s="29">
         <v>2</v>
@@ -25154,7 +25161,7 @@
         <v>15</v>
       </c>
       <c r="G80" s="28" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H80" s="31" t="s">
         <v>15</v>
@@ -25183,13 +25190,13 @@
         <v>97</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C81" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D81" s="28" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E81" s="29">
         <v>4</v>
@@ -25198,7 +25205,7 @@
         <v>15</v>
       </c>
       <c r="G81" s="28" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="H81" s="31" t="s">
         <v>15</v>
@@ -25227,13 +25234,13 @@
         <v>98</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C82" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D82" s="28" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E82" s="29">
         <v>7</v>
@@ -25242,7 +25249,7 @@
         <v>15</v>
       </c>
       <c r="G82" s="28" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="H82" s="31" t="s">
         <v>15</v>
@@ -25271,13 +25278,13 @@
         <v>99</v>
       </c>
       <c r="B83" s="26" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C83" s="27" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D83" s="28" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E83" s="29">
         <v>2</v>
@@ -25286,7 +25293,7 @@
         <v>15</v>
       </c>
       <c r="G83" s="28" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="H83" s="31" t="s">
         <v>15</v>
@@ -25315,13 +25322,13 @@
         <v>100</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C84" s="27" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D84" s="28" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E84" s="29">
         <v>2</v>
@@ -25330,7 +25337,7 @@
         <v>15</v>
       </c>
       <c r="G84" s="28" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="H84" s="31" t="s">
         <v>15</v>
@@ -25359,13 +25366,13 @@
         <v>101</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C85" s="27" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D85" s="28" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E85" s="29">
         <v>2</v>
@@ -25374,7 +25381,7 @@
         <v>15</v>
       </c>
       <c r="G85" s="28" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="H85" s="31" t="s">
         <v>15</v>
@@ -25403,7 +25410,7 @@
         <v>102</v>
       </c>
       <c r="B86" s="26" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C86" s="27" t="s">
         <v>173</v>
@@ -25418,7 +25425,7 @@
         <v>15</v>
       </c>
       <c r="G86" s="28" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="H86" s="31" t="s">
         <v>15</v>
@@ -25447,22 +25454,22 @@
         <v>103</v>
       </c>
       <c r="B87" s="26" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C87" s="27" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D87" s="28" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E87" s="29">
         <v>4</v>
       </c>
       <c r="F87" s="30" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="G87" s="28" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="H87" s="31" t="s">
         <v>15</v>
@@ -25491,10 +25498,10 @@
         <v>104</v>
       </c>
       <c r="B88" s="26" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C88" s="27" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D88" s="28" t="s">
         <v>15</v>
@@ -25506,7 +25513,7 @@
         <v>15</v>
       </c>
       <c r="G88" s="28" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="H88" s="31" t="s">
         <v>15</v>
@@ -25532,7 +25539,7 @@
     </row>
     <row r="89" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="97" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B89" s="26" t="s">
         <v>15</v>
@@ -25615,13 +25622,13 @@
         <v>108</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C91" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D91" s="28" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E91" s="29">
         <v>1</v>
@@ -25630,7 +25637,7 @@
         <v>188</v>
       </c>
       <c r="G91" s="28" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="H91" s="31" t="s">
         <v>15</v>
@@ -25659,13 +25666,13 @@
         <v>109</v>
       </c>
       <c r="B92" s="26" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C92" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D92" s="28" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E92" s="29">
         <v>1</v>
@@ -25674,7 +25681,7 @@
         <v>188</v>
       </c>
       <c r="G92" s="28" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="H92" s="31" t="s">
         <v>15</v>
@@ -25703,13 +25710,13 @@
         <v>110</v>
       </c>
       <c r="B93" s="26" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C93" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D93" s="28" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E93" s="29">
         <v>2</v>
@@ -25718,7 +25725,7 @@
         <v>192</v>
       </c>
       <c r="G93" s="28" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="H93" s="31" t="s">
         <v>15</v>
@@ -25747,13 +25754,13 @@
         <v>111</v>
       </c>
       <c r="B94" s="26" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C94" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E94" s="29">
         <v>2</v>
@@ -25762,7 +25769,7 @@
         <v>192</v>
       </c>
       <c r="G94" s="28" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="H94" s="31" t="s">
         <v>15</v>
@@ -25791,13 +25798,13 @@
         <v>112</v>
       </c>
       <c r="B95" s="26" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C95" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D95" s="28" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E95" s="29">
         <v>3</v>
@@ -25806,7 +25813,7 @@
         <v>200</v>
       </c>
       <c r="G95" s="28" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="H95" s="31" t="s">
         <v>15</v>
@@ -25835,13 +25842,13 @@
         <v>113</v>
       </c>
       <c r="B96" s="26" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C96" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D96" s="28" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E96" s="29">
         <v>4</v>
@@ -25850,7 +25857,7 @@
         <v>213</v>
       </c>
       <c r="G96" s="28" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="H96" s="31" t="s">
         <v>15</v>
@@ -25879,13 +25886,13 @@
         <v>114</v>
       </c>
       <c r="B97" s="26" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C97" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D97" s="28" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E97" s="29">
         <v>4</v>
@@ -25894,7 +25901,7 @@
         <v>213</v>
       </c>
       <c r="G97" s="28" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="H97" s="31" t="s">
         <v>15</v>
@@ -25923,7 +25930,7 @@
         <v>115</v>
       </c>
       <c r="B98" s="26" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C98" s="27" t="s">
         <v>186</v>
@@ -25935,13 +25942,13 @@
         <v>6</v>
       </c>
       <c r="F98" s="30" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G98" s="28" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="H98" s="31" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="I98" s="28"/>
       <c r="J98" s="27"/>
@@ -25967,22 +25974,22 @@
         <v>116</v>
       </c>
       <c r="B99" s="26" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C99" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D99" s="28" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="E99" s="29">
         <v>15</v>
       </c>
       <c r="F99" s="30" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G99" s="28" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="H99" s="31" t="s">
         <v>15</v>
@@ -26011,13 +26018,13 @@
         <v>117</v>
       </c>
       <c r="B100" s="26" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C100" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D100" s="28" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E100" s="29">
         <v>1</v>
@@ -26026,7 +26033,7 @@
         <v>15</v>
       </c>
       <c r="G100" s="28" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="H100" s="31" t="s">
         <v>15</v>
@@ -26055,13 +26062,13 @@
         <v>118</v>
       </c>
       <c r="B101" s="26" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C101" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D101" s="28" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E101" s="29">
         <v>1</v>
@@ -26070,7 +26077,7 @@
         <v>15</v>
       </c>
       <c r="G101" s="28" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="H101" s="31" t="s">
         <v>15</v>
@@ -26099,13 +26106,13 @@
         <v>119</v>
       </c>
       <c r="B102" s="26" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C102" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D102" s="28" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E102" s="29">
         <v>1</v>
@@ -26114,7 +26121,7 @@
         <v>15</v>
       </c>
       <c r="G102" s="28" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="H102" s="31" t="s">
         <v>15</v>
@@ -26143,13 +26150,13 @@
         <v>120</v>
       </c>
       <c r="B103" s="26" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C103" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D103" s="28" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E103" s="29">
         <v>2</v>
@@ -26158,7 +26165,7 @@
         <v>15</v>
       </c>
       <c r="G103" s="28" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="H103" s="31" t="s">
         <v>15</v>
@@ -26187,13 +26194,13 @@
         <v>121</v>
       </c>
       <c r="B104" s="26" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C104" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D104" s="28" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E104" s="29">
         <v>2</v>
@@ -26202,7 +26209,7 @@
         <v>15</v>
       </c>
       <c r="G104" s="28" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H104" s="31" t="s">
         <v>15</v>
@@ -26231,13 +26238,13 @@
         <v>122</v>
       </c>
       <c r="B105" s="26" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C105" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D105" s="28" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E105" s="29">
         <v>4</v>
@@ -26246,7 +26253,7 @@
         <v>15</v>
       </c>
       <c r="G105" s="28" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="H105" s="31" t="s">
         <v>15</v>
@@ -26275,13 +26282,13 @@
         <v>123</v>
       </c>
       <c r="B106" s="26" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C106" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D106" s="28" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E106" s="29">
         <v>7</v>
@@ -26290,7 +26297,7 @@
         <v>15</v>
       </c>
       <c r="G106" s="28" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="H106" s="31" t="s">
         <v>15</v>
@@ -26319,13 +26326,13 @@
         <v>124</v>
       </c>
       <c r="B107" s="26" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C107" s="27" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D107" s="28" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E107" s="29">
         <v>2</v>
@@ -26334,7 +26341,7 @@
         <v>15</v>
       </c>
       <c r="G107" s="28" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="H107" s="31" t="s">
         <v>15</v>
@@ -26363,13 +26370,13 @@
         <v>125</v>
       </c>
       <c r="B108" s="26" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C108" s="27" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D108" s="28" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E108" s="29">
         <v>2</v>
@@ -26378,7 +26385,7 @@
         <v>15</v>
       </c>
       <c r="G108" s="28" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="H108" s="31" t="s">
         <v>15</v>
@@ -26407,7 +26414,7 @@
         <v>126</v>
       </c>
       <c r="B109" s="26" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C109" s="27" t="s">
         <v>173</v>
@@ -26422,7 +26429,7 @@
         <v>15</v>
       </c>
       <c r="G109" s="28" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="H109" s="31" t="s">
         <v>15</v>
@@ -26451,10 +26458,10 @@
         <v>127</v>
       </c>
       <c r="B110" s="26" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C110" s="27" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D110" s="28" t="s">
         <v>15</v>
@@ -26466,7 +26473,7 @@
         <v>15</v>
       </c>
       <c r="G110" s="28" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="H110" s="31" t="s">
         <v>15</v>
@@ -26492,7 +26499,7 @@
     </row>
     <row r="111" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="97" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B111" s="26" t="s">
         <v>15</v>
@@ -26575,7 +26582,7 @@
         <v>131</v>
       </c>
       <c r="B113" s="26" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C113" s="27" t="s">
         <v>186</v>
@@ -26587,10 +26594,10 @@
         <v>1</v>
       </c>
       <c r="F113" s="30" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G113" s="28" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="H113" s="31" t="s">
         <v>15</v>
@@ -26619,7 +26626,7 @@
         <v>132</v>
       </c>
       <c r="B114" s="26" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C114" s="27" t="s">
         <v>186</v>
@@ -26637,7 +26644,7 @@
         <v>16</v>
       </c>
       <c r="H114" s="31" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="I114" s="28"/>
       <c r="J114" s="27"/>
@@ -26663,7 +26670,7 @@
         <v>133</v>
       </c>
       <c r="B115" s="26" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C115" s="27" t="s">
         <v>186</v>
@@ -26678,7 +26685,7 @@
         <v>192</v>
       </c>
       <c r="G115" s="28" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="H115" s="31" t="s">
         <v>15</v>
@@ -26707,7 +26714,7 @@
         <v>134</v>
       </c>
       <c r="B116" s="26" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C116" s="27" t="s">
         <v>186</v>
@@ -26722,7 +26729,7 @@
         <v>213</v>
       </c>
       <c r="G116" s="28" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="H116" s="31" t="s">
         <v>15</v>
@@ -26751,7 +26758,7 @@
         <v>135</v>
       </c>
       <c r="B117" s="26" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C117" s="27" t="s">
         <v>186</v>
@@ -26766,7 +26773,7 @@
         <v>192</v>
       </c>
       <c r="G117" s="28" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="H117" s="31" t="s">
         <v>15</v>
@@ -26795,13 +26802,13 @@
         <v>136</v>
       </c>
       <c r="B118" s="26" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C118" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D118" s="28" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="E118" s="29">
         <v>3</v>
@@ -26810,7 +26817,7 @@
         <v>188</v>
       </c>
       <c r="G118" s="28" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="H118" s="31" t="s">
         <v>15</v>
@@ -26839,13 +26846,13 @@
         <v>137</v>
       </c>
       <c r="B119" s="26" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C119" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D119" s="28" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E119" s="29">
         <v>4</v>
@@ -26854,7 +26861,7 @@
         <v>200</v>
       </c>
       <c r="G119" s="28" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="H119" s="31" t="s">
         <v>15</v>
@@ -26883,7 +26890,7 @@
         <v>138</v>
       </c>
       <c r="B120" s="26" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C120" s="27" t="s">
         <v>186</v>
@@ -26895,13 +26902,13 @@
         <v>4</v>
       </c>
       <c r="F120" s="30" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="G120" s="28" t="s">
         <v>16</v>
       </c>
       <c r="H120" s="31" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="I120" s="28"/>
       <c r="J120" s="27"/>
@@ -26927,7 +26934,7 @@
         <v>139</v>
       </c>
       <c r="B121" s="26" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C121" s="27" t="s">
         <v>186</v>
@@ -26939,10 +26946,10 @@
         <v>5</v>
       </c>
       <c r="F121" s="30" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="G121" s="28" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="H121" s="31" t="s">
         <v>15</v>
@@ -26971,22 +26978,22 @@
         <v>140</v>
       </c>
       <c r="B122" s="26" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C122" s="27" t="s">
         <v>186</v>
       </c>
       <c r="D122" s="28" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E122" s="29">
         <v>20</v>
       </c>
       <c r="F122" s="30" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G122" s="28" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="H122" s="31" t="s">
         <v>15</v>
@@ -27015,13 +27022,13 @@
         <v>141</v>
       </c>
       <c r="B123" s="26" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C123" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D123" s="28" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E123" s="29">
         <v>1</v>
@@ -27030,7 +27037,7 @@
         <v>188</v>
       </c>
       <c r="G123" s="28" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="H123" s="31" t="s">
         <v>15</v>
@@ -27059,13 +27066,13 @@
         <v>142</v>
       </c>
       <c r="B124" s="26" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C124" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D124" s="28" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E124" s="29">
         <v>1</v>
@@ -27074,7 +27081,7 @@
         <v>188</v>
       </c>
       <c r="G124" s="28" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="H124" s="31" t="s">
         <v>15</v>
@@ -27103,13 +27110,13 @@
         <v>143</v>
       </c>
       <c r="B125" s="26" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C125" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D125" s="28" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E125" s="29">
         <v>1</v>
@@ -27118,7 +27125,7 @@
         <v>15</v>
       </c>
       <c r="G125" s="28" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="H125" s="31" t="s">
         <v>15</v>
@@ -27147,13 +27154,13 @@
         <v>144</v>
       </c>
       <c r="B126" s="26" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C126" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D126" s="28" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E126" s="29">
         <v>1</v>
@@ -27162,7 +27169,7 @@
         <v>188</v>
       </c>
       <c r="G126" s="28" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H126" s="31" t="s">
         <v>15</v>
@@ -27191,13 +27198,13 @@
         <v>145</v>
       </c>
       <c r="B127" s="26" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C127" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D127" s="28" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E127" s="29">
         <v>2</v>
@@ -27206,7 +27213,7 @@
         <v>188</v>
       </c>
       <c r="G127" s="28" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="H127" s="31" t="s">
         <v>15</v>
@@ -27235,13 +27242,13 @@
         <v>146</v>
       </c>
       <c r="B128" s="26" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C128" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D128" s="28" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E128" s="29">
         <v>2</v>
@@ -27250,7 +27257,7 @@
         <v>188</v>
       </c>
       <c r="G128" s="28" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="H128" s="31" t="s">
         <v>15</v>
@@ -27279,13 +27286,13 @@
         <v>147</v>
       </c>
       <c r="B129" s="26" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C129" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D129" s="28" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E129" s="29">
         <v>3</v>
@@ -27294,7 +27301,7 @@
         <v>188</v>
       </c>
       <c r="G129" s="28" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="H129" s="31" t="s">
         <v>15</v>
@@ -27323,10 +27330,10 @@
         <v>148</v>
       </c>
       <c r="B130" s="26" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C130" s="27" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D130" s="28" t="s">
         <v>226</v>
@@ -27338,7 +27345,7 @@
         <v>15</v>
       </c>
       <c r="G130" s="28" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="H130" s="31" t="s">
         <v>15</v>
@@ -27367,13 +27374,13 @@
         <v>149</v>
       </c>
       <c r="B131" s="26" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C131" s="27" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D131" s="28" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E131" s="29">
         <v>2</v>
@@ -27382,7 +27389,7 @@
         <v>15</v>
       </c>
       <c r="G131" s="28" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="H131" s="31" t="s">
         <v>15</v>
@@ -27411,7 +27418,7 @@
         <v>150</v>
       </c>
       <c r="B132" s="26" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C132" s="27" t="s">
         <v>173</v>
@@ -27426,7 +27433,7 @@
         <v>15</v>
       </c>
       <c r="G132" s="28" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="H132" s="31" t="s">
         <v>15</v>
@@ -27452,7 +27459,7 @@
     </row>
     <row r="133" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="99" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B133" s="26" t="s">
         <v>15</v>
@@ -27531,7 +27538,7 @@
         <v>152</v>
       </c>
       <c r="B135" s="26" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C135" s="27" t="s">
         <v>186</v>
@@ -27546,7 +27553,7 @@
         <v>188</v>
       </c>
       <c r="G135" s="28" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="H135" s="31" t="s">
         <v>15</v>
@@ -27575,7 +27582,7 @@
         <v>153</v>
       </c>
       <c r="B136" s="26" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C136" s="27" t="s">
         <v>186</v>
@@ -27587,10 +27594,10 @@
         <v>3</v>
       </c>
       <c r="F136" s="30" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G136" s="28" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="H136" s="31" t="s">
         <v>15</v>
@@ -27619,7 +27626,7 @@
         <v>154</v>
       </c>
       <c r="B137" s="26" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C137" s="27" t="s">
         <v>186</v>
@@ -27631,10 +27638,10 @@
         <v>3</v>
       </c>
       <c r="F137" s="30" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G137" s="28" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="H137" s="31" t="s">
         <v>202</v>
@@ -27663,7 +27670,7 @@
         <v>155</v>
       </c>
       <c r="B138" s="26" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C138" s="27" t="s">
         <v>186</v>
@@ -27678,7 +27685,7 @@
         <v>213</v>
       </c>
       <c r="G138" s="28" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="H138" s="31" t="s">
         <v>15</v>
@@ -27707,7 +27714,7 @@
         <v>156</v>
       </c>
       <c r="B139" s="26" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C139" s="27" t="s">
         <v>186</v>
@@ -27719,10 +27726,10 @@
         <v>4</v>
       </c>
       <c r="F139" s="30" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="G139" s="28" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="H139" s="31" t="s">
         <v>15</v>
@@ -27751,7 +27758,7 @@
         <v>157</v>
       </c>
       <c r="B140" s="26" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C140" s="27" t="s">
         <v>186</v>
@@ -27763,10 +27770,10 @@
         <v>5</v>
       </c>
       <c r="F140" s="30" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="G140" s="28" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="H140" s="31" t="s">
         <v>202</v>
@@ -27795,13 +27802,13 @@
         <v>158</v>
       </c>
       <c r="B141" s="26" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C141" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D141" s="28" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E141" s="29">
         <v>1</v>
@@ -27810,7 +27817,7 @@
         <v>15</v>
       </c>
       <c r="G141" s="28" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="H141" s="31" t="s">
         <v>15</v>
@@ -27839,13 +27846,13 @@
         <v>159</v>
       </c>
       <c r="B142" s="26" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C142" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D142" s="28" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E142" s="29">
         <v>3</v>
@@ -27854,7 +27861,7 @@
         <v>15</v>
       </c>
       <c r="G142" s="28" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="H142" s="31" t="s">
         <v>15</v>
@@ -27883,13 +27890,13 @@
         <v>160</v>
       </c>
       <c r="B143" s="26" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C143" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D143" s="28" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E143" s="29">
         <v>3</v>
@@ -27898,7 +27905,7 @@
         <v>15</v>
       </c>
       <c r="G143" s="28" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="H143" s="31" t="s">
         <v>15</v>
@@ -27927,13 +27934,13 @@
         <v>161</v>
       </c>
       <c r="B144" s="26" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C144" s="27" t="s">
         <v>225</v>
       </c>
       <c r="D144" s="28" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E144" s="29">
         <v>4</v>
@@ -27942,7 +27949,7 @@
         <v>15</v>
       </c>
       <c r="G144" s="28" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="H144" s="31" t="s">
         <v>15</v>
@@ -27968,7 +27975,7 @@
     </row>
     <row r="145" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="99" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B145" s="26" t="s">
         <v>15</v>
@@ -28012,7 +28019,7 @@
     </row>
     <row r="146" spans="1:26" s="100" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="101" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B146" s="101"/>
       <c r="C146" s="101"/>
@@ -28352,7 +28359,7 @@
     </row>
     <row r="154" spans="1:26" s="105" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="106" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B154" s="106"/>
       <c r="C154" s="106"/>
@@ -28384,7 +28391,7 @@
     </row>
     <row r="155" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="99" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B155" s="26" t="s">
         <v>15</v>

</xml_diff>